<commit_message>
Cleaned up and added comments
Still need to implement save function and add appointment function
</commit_message>
<xml_diff>
--- a/exampleTable.xlsx
+++ b/exampleTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace_Eclipse\appointmentBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4772DFCB-DE42-4D0C-BF29-980059C35A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCEB6BA-3E43-4C9D-ACAF-4F3022B536F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A0A3309-AEB1-4D6A-BD2A-827387067543}"/>
   </bookViews>
@@ -598,7 +598,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +606,7 @@
     <col min="3" max="3" width="9.140625" style="2"/>
     <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>